<commit_message>
updates on the benchmark
</commit_message>
<xml_diff>
--- a/doc/Score summary20210307.xlsx
+++ b/doc/Score summary20210307.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UW\directproject\dev\dummydata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UW\directproject\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB635D2B-4FEC-4860-9F01-10E75098E29C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E6048C-2781-47A7-AEF8-C4863259439E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -1675,7 +1675,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
-          <c:min val="0.9"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -7004,20 +7004,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -7066,20 +7052,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -7392,20 +7364,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -7454,20 +7412,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -15055,15 +14999,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -15091,16 +15035,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>314324</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15547,8 +15491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Y11" sqref="Y11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Z6" sqref="Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -16506,7 +16450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3479E86A-85FA-4496-BE21-2F8C57CDB9CC}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -16516,7 +16460,7 @@
     <col min="3" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -17010,7 +16954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
         <v>0</v>
       </c>
@@ -17433,8 +17377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C35BC272-F1DE-4D4E-8FFF-F3C1F2832E6A}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -17444,7 +17388,7 @@
     <col min="3" max="8" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="9" t="s">
         <v>114</v>
       </c>
@@ -17468,7 +17412,7 @@
       </c>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>46</v>
       </c>
@@ -17494,7 +17438,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>47</v>
       </c>
@@ -17572,7 +17516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>53</v>
       </c>
@@ -17598,7 +17542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>54</v>
       </c>
@@ -17624,7 +17568,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>55</v>
       </c>
@@ -17650,7 +17594,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>56</v>
       </c>
@@ -17676,7 +17620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>57</v>
       </c>
@@ -17702,7 +17646,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>58</v>
       </c>
@@ -17728,7 +17672,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>59</v>
       </c>
@@ -17754,7 +17698,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>60</v>
       </c>
@@ -17780,7 +17724,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>61</v>
       </c>
@@ -17806,7 +17750,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>62</v>
       </c>
@@ -17832,7 +17776,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>63</v>
       </c>
@@ -17870,7 +17814,7 @@
   <dimension ref="A1:I119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>